<commit_message>
Deleting a sheet in the Excel ReverseSortedInput.xlsx
</commit_message>
<xml_diff>
--- a/ReverseSortedInput.xlsx
+++ b/ReverseSortedInput.xlsx
@@ -14,7 +14,6 @@
   <sheets>
     <sheet name="Reverse Sorted Input Data" sheetId="1" r:id="rId1"/>
     <sheet name="Average of the Input Data" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet1" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -116,10 +115,10 @@
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -612,7 +611,7 @@
       <c r="A12" s="1">
         <v>1000</v>
       </c>
-      <c r="B12" s="3" t="s">
+      <c r="B12" s="2" t="s">
         <v>9</v>
       </c>
       <c r="C12" s="1">
@@ -879,7 +878,7 @@
       <c r="A24" s="1">
         <v>2000</v>
       </c>
-      <c r="B24" s="3" t="s">
+      <c r="B24" s="2" t="s">
         <v>9</v>
       </c>
       <c r="C24" s="1">
@@ -1146,7 +1145,7 @@
       <c r="A36" s="1">
         <v>3000</v>
       </c>
-      <c r="B36" s="3" t="s">
+      <c r="B36" s="2" t="s">
         <v>9</v>
       </c>
       <c r="C36" s="1">
@@ -1413,7 +1412,7 @@
       <c r="A48" s="1">
         <v>4000</v>
       </c>
-      <c r="B48" s="3" t="s">
+      <c r="B48" s="2" t="s">
         <v>9</v>
       </c>
       <c r="C48" s="1">
@@ -1680,7 +1679,7 @@
       <c r="A60" s="1">
         <v>5000</v>
       </c>
-      <c r="B60" s="3" t="s">
+      <c r="B60" s="2" t="s">
         <v>9</v>
       </c>
       <c r="C60" s="1">
@@ -1947,7 +1946,7 @@
       <c r="A72" s="1">
         <v>10000</v>
       </c>
-      <c r="B72" s="3" t="s">
+      <c r="B72" s="2" t="s">
         <v>9</v>
       </c>
       <c r="C72" s="1">
@@ -2214,7 +2213,7 @@
       <c r="A84" s="1">
         <v>20000</v>
       </c>
-      <c r="B84" s="3" t="s">
+      <c r="B84" s="2" t="s">
         <v>9</v>
       </c>
       <c r="C84" s="1">
@@ -2481,7 +2480,7 @@
       <c r="A96" s="1">
         <v>40000</v>
       </c>
-      <c r="B96" s="3" t="s">
+      <c r="B96" s="2" t="s">
         <v>9</v>
       </c>
       <c r="C96" s="1">
@@ -2748,7 +2747,7 @@
       <c r="A108" s="1">
         <v>50000</v>
       </c>
-      <c r="B108" s="3" t="s">
+      <c r="B108" s="2" t="s">
         <v>9</v>
       </c>
       <c r="C108" s="1">
@@ -3015,7 +3014,7 @@
       <c r="A120" s="1">
         <v>60000</v>
       </c>
-      <c r="B120" s="3" t="s">
+      <c r="B120" s="2" t="s">
         <v>9</v>
       </c>
       <c r="C120" s="1">
@@ -3282,7 +3281,7 @@
       <c r="A132" s="1">
         <v>80000</v>
       </c>
-      <c r="B132" s="3" t="s">
+      <c r="B132" s="2" t="s">
         <v>9</v>
       </c>
       <c r="C132" s="1">
@@ -3549,7 +3548,7 @@
       <c r="A144" s="1">
         <v>90000</v>
       </c>
-      <c r="B144" s="3" t="s">
+      <c r="B144" s="2" t="s">
         <v>9</v>
       </c>
       <c r="C144" s="1">
@@ -3816,7 +3815,7 @@
       <c r="A156" s="1">
         <v>100000</v>
       </c>
-      <c r="B156" s="3" t="s">
+      <c r="B156" s="2" t="s">
         <v>9</v>
       </c>
       <c r="C156" s="1">
@@ -4734,32 +4733,32 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="13" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
     </row>
     <row r="2" spans="1:6" ht="13" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="F2" s="2" t="s">
         <v>6</v>
       </c>
     </row>
@@ -5024,32 +5023,32 @@
       </c>
     </row>
     <row r="17" spans="1:6" ht="13" x14ac:dyDescent="0.25">
-      <c r="A17" s="2" t="s">
+      <c r="A17" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B17" s="2"/>
-      <c r="C17" s="2"/>
-      <c r="D17" s="2"/>
-      <c r="E17" s="2"/>
-      <c r="F17" s="2"/>
+      <c r="B17" s="3"/>
+      <c r="C17" s="3"/>
+      <c r="D17" s="3"/>
+      <c r="E17" s="3"/>
+      <c r="F17" s="3"/>
     </row>
     <row r="18" spans="1:6" ht="13" x14ac:dyDescent="0.25">
-      <c r="A18" s="3" t="s">
+      <c r="A18" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B18" s="3" t="s">
+      <c r="B18" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C18" s="3" t="s">
+      <c r="C18" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D18" s="3" t="s">
+      <c r="D18" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E18" s="3" t="s">
+      <c r="E18" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="F18" s="3" t="s">
+      <c r="F18" s="2" t="s">
         <v>6</v>
       </c>
     </row>
@@ -5385,18 +5384,4 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:F2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>